<commit_message>
added reporting with datasets
</commit_message>
<xml_diff>
--- a/MappingAndReporting/resources/Participants.xlsx
+++ b/MappingAndReporting/resources/Participants.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\yardsales\mapping\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\yardsales\MappingAndReporting\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7807E184-446C-4E28-A6FC-087A441AF28E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63F842D3-AB7C-4E71-B0D3-870363944974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5160" yWindow="750" windowWidth="25995" windowHeight="16290" xr2:uid="{2342445F-2DC2-4AC9-B0F7-98DE2CF4F4DA}"/>
+    <workbookView xWindow="5505" yWindow="1095" windowWidth="25995" windowHeight="16290" xr2:uid="{2342445F-2DC2-4AC9-B0F7-98DE2CF4F4DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="__Q__">Report!$A$11:$AI$12</definedName>
+    <definedName name="__P__">Report!$A$11:$AI$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,16 +44,16 @@
     <t>&lt;#YardSaleTitle&gt;</t>
   </si>
   <si>
-    <t>&lt;#Q.Name&gt;</t>
+    <t>&lt;#YardSaleEventDates&gt;</t>
   </si>
   <si>
-    <t>&lt;#Q.Address&gt;</t>
+    <t>&lt;#P.Name&gt;</t>
   </si>
   <si>
-    <t>&lt;#Q.Categories&gt;</t>
+    <t>&lt;#P.Address&gt;</t>
   </si>
   <si>
-    <t>&lt;#YardSaleDates&gt;</t>
+    <t>&lt;#P.Categories&gt;</t>
   </si>
 </sst>
 </file>
@@ -149,17 +149,17 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -527,7 +527,7 @@
   <dimension ref="A1:AT20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,41 +539,41 @@
   <sheetData>
     <row r="1" spans="1:46" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8"/>
-      <c r="W1" s="8"/>
-      <c r="X1" s="8"/>
-      <c r="Y1" s="8"/>
-      <c r="Z1" s="8"/>
-      <c r="AA1" s="8"/>
-      <c r="AB1" s="8"/>
-      <c r="AC1" s="8"/>
-      <c r="AD1" s="8"/>
-      <c r="AE1" s="8"/>
-      <c r="AF1" s="8"/>
-      <c r="AG1" s="8"/>
-      <c r="AH1" s="8"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
+      <c r="AA1" s="6"/>
+      <c r="AB1" s="6"/>
+      <c r="AC1" s="6"/>
+      <c r="AD1" s="6"/>
+      <c r="AE1" s="6"/>
+      <c r="AF1" s="6"/>
+      <c r="AG1" s="6"/>
+      <c r="AH1" s="6"/>
       <c r="AI1" s="3"/>
       <c r="AJ1" s="3"/>
       <c r="AK1" s="3"/>
@@ -589,41 +589,41 @@
     </row>
     <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
-      <c r="B2" s="9" t="s">
-        <v>4</v>
+      <c r="B2" s="7" t="s">
+        <v>1</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9"/>
-      <c r="U2" s="9"/>
-      <c r="V2" s="9"/>
-      <c r="W2" s="9"/>
-      <c r="X2" s="9"/>
-      <c r="Y2" s="9"/>
-      <c r="Z2" s="9"/>
-      <c r="AA2" s="9"/>
-      <c r="AB2" s="9"/>
-      <c r="AC2" s="9"/>
-      <c r="AD2" s="9"/>
-      <c r="AE2" s="9"/>
-      <c r="AF2" s="9"/>
-      <c r="AG2" s="9"/>
-      <c r="AH2" s="9"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="7"/>
+      <c r="X2" s="7"/>
+      <c r="Y2" s="7"/>
+      <c r="Z2" s="7"/>
+      <c r="AA2" s="7"/>
+      <c r="AB2" s="7"/>
+      <c r="AC2" s="7"/>
+      <c r="AD2" s="7"/>
+      <c r="AE2" s="7"/>
+      <c r="AF2" s="7"/>
+      <c r="AG2" s="7"/>
+      <c r="AH2" s="7"/>
       <c r="AI2" s="3"/>
       <c r="AJ2" s="3"/>
       <c r="AK2" s="3"/>
@@ -1023,43 +1023,43 @@
     </row>
     <row r="11" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
-      <c r="B11" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6" t="s">
+      <c r="B11" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="6"/>
-      <c r="S11" s="6"/>
-      <c r="T11" s="6"/>
-      <c r="U11" s="6"/>
-      <c r="V11" s="6"/>
-      <c r="W11" s="6"/>
-      <c r="X11" s="6"/>
-      <c r="Y11" s="6"/>
-      <c r="Z11" s="6"/>
-      <c r="AA11" s="6"/>
-      <c r="AB11" s="6"/>
-      <c r="AC11" s="6"/>
-      <c r="AD11" s="6"/>
-      <c r="AE11" s="6"/>
-      <c r="AF11" s="6"/>
-      <c r="AG11" s="6"/>
-      <c r="AH11" s="6"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="8"/>
+      <c r="T11" s="8"/>
+      <c r="U11" s="8"/>
+      <c r="V11" s="8"/>
+      <c r="W11" s="8"/>
+      <c r="X11" s="8"/>
+      <c r="Y11" s="8"/>
+      <c r="Z11" s="8"/>
+      <c r="AA11" s="8"/>
+      <c r="AB11" s="8"/>
+      <c r="AC11" s="8"/>
+      <c r="AD11" s="8"/>
+      <c r="AE11" s="8"/>
+      <c r="AF11" s="8"/>
+      <c r="AG11" s="8"/>
+      <c r="AH11" s="8"/>
       <c r="AI11" s="3"/>
       <c r="AJ11" s="3"/>
       <c r="AK11" s="3"/>
@@ -1077,39 +1077,39 @@
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="7" t="s">
-        <v>3</v>
+      <c r="D12" s="9" t="s">
+        <v>4</v>
       </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="7"/>
-      <c r="S12" s="7"/>
-      <c r="T12" s="7"/>
-      <c r="U12" s="7"/>
-      <c r="V12" s="7"/>
-      <c r="W12" s="7"/>
-      <c r="X12" s="7"/>
-      <c r="Y12" s="7"/>
-      <c r="Z12" s="7"/>
-      <c r="AA12" s="7"/>
-      <c r="AB12" s="7"/>
-      <c r="AC12" s="7"/>
-      <c r="AD12" s="7"/>
-      <c r="AE12" s="7"/>
-      <c r="AF12" s="7"/>
-      <c r="AG12" s="7"/>
-      <c r="AH12" s="7"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="9"/>
+      <c r="V12" s="9"/>
+      <c r="W12" s="9"/>
+      <c r="X12" s="9"/>
+      <c r="Y12" s="9"/>
+      <c r="Z12" s="9"/>
+      <c r="AA12" s="9"/>
+      <c r="AB12" s="9"/>
+      <c r="AC12" s="9"/>
+      <c r="AD12" s="9"/>
+      <c r="AE12" s="9"/>
+      <c r="AF12" s="9"/>
+      <c r="AG12" s="9"/>
+      <c r="AH12" s="9"/>
       <c r="AI12" s="3"/>
       <c r="AJ12" s="3"/>
       <c r="AK12" s="3"/>

</xml_diff>